<commit_message>
Update schedule file: Y3_B2526_Urogenital_schedule.xlsx
</commit_message>
<xml_diff>
--- a/modules_schedules/Y3_B2526_Urogenital_schedule.xlsx
+++ b/modules_schedules/Y3_B2526_Urogenital_schedule.xlsx
@@ -463,7 +463,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G83"/>
+  <dimension ref="A1:G115"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -565,22 +565,22 @@
       </c>
       <c r="C3" s="6" t="inlineStr">
         <is>
-          <t>biochemistry lab/cbl</t>
+          <t>anatomy</t>
         </is>
       </c>
       <c r="D3" s="6" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>2</t>
         </is>
       </c>
       <c r="E3" s="7" t="inlineStr">
         <is>
-          <t>13/11/2025</t>
+          <t>09/12/2025</t>
         </is>
       </c>
       <c r="F3" s="8" t="inlineStr">
         <is>
-          <t>12:00:00</t>
+          <t>08:00:00</t>
         </is>
       </c>
       <c r="G3" s="9" t="n">
@@ -600,22 +600,22 @@
       </c>
       <c r="C4" s="2" t="inlineStr">
         <is>
-          <t>histology</t>
+          <t>anatomy</t>
         </is>
       </c>
       <c r="D4" s="2" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>3</t>
         </is>
       </c>
       <c r="E4" s="3" t="inlineStr">
         <is>
-          <t>11/11/2025</t>
+          <t>15/12/2025</t>
         </is>
       </c>
       <c r="F4" s="4" t="inlineStr">
         <is>
-          <t>10:00:00</t>
+          <t>12:00:00</t>
         </is>
       </c>
       <c r="G4" s="5" t="n">
@@ -635,17 +635,17 @@
       </c>
       <c r="C5" s="6" t="inlineStr">
         <is>
-          <t>histology</t>
+          <t>biochemistry lab/cbl</t>
         </is>
       </c>
       <c r="D5" s="6" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>1</t>
         </is>
       </c>
       <c r="E5" s="7" t="inlineStr">
         <is>
-          <t>04/12/2025</t>
+          <t>13/11/2025</t>
         </is>
       </c>
       <c r="F5" s="8" t="inlineStr">
@@ -670,7 +670,7 @@
       </c>
       <c r="C6" s="2" t="inlineStr">
         <is>
-          <t>microbiology</t>
+          <t>histology</t>
         </is>
       </c>
       <c r="D6" s="2" t="inlineStr">
@@ -680,12 +680,12 @@
       </c>
       <c r="E6" s="3" t="inlineStr">
         <is>
-          <t>26/11/2025</t>
+          <t>11/11/2025</t>
         </is>
       </c>
       <c r="F6" s="4" t="inlineStr">
         <is>
-          <t>12:00:00</t>
+          <t>10:00:00</t>
         </is>
       </c>
       <c r="G6" s="5" t="n">
@@ -705,7 +705,7 @@
       </c>
       <c r="C7" s="6" t="inlineStr">
         <is>
-          <t>microbiology</t>
+          <t>histology</t>
         </is>
       </c>
       <c r="D7" s="6" t="inlineStr">
@@ -715,12 +715,12 @@
       </c>
       <c r="E7" s="7" t="inlineStr">
         <is>
-          <t>08/12/2025</t>
+          <t>04/12/2025</t>
         </is>
       </c>
       <c r="F7" s="8" t="inlineStr">
         <is>
-          <t>14:00:00</t>
+          <t>12:00:00</t>
         </is>
       </c>
       <c r="G7" s="9" t="n">
@@ -740,22 +740,22 @@
       </c>
       <c r="C8" s="2" t="inlineStr">
         <is>
-          <t>parasitology sgd/pos</t>
+          <t>histology</t>
         </is>
       </c>
       <c r="D8" s="2" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>3</t>
         </is>
       </c>
       <c r="E8" s="3" t="inlineStr">
         <is>
-          <t>11/12/2025</t>
+          <t>14/12/2025</t>
         </is>
       </c>
       <c r="F8" s="4" t="inlineStr">
         <is>
-          <t>14:00:00</t>
+          <t>10:00:00</t>
         </is>
       </c>
       <c r="G8" s="5" t="n">
@@ -775,7 +775,7 @@
       </c>
       <c r="C9" s="6" t="inlineStr">
         <is>
-          <t>pathology lab/museum</t>
+          <t>microbiology</t>
         </is>
       </c>
       <c r="D9" s="6" t="inlineStr">
@@ -785,12 +785,12 @@
       </c>
       <c r="E9" s="7" t="inlineStr">
         <is>
-          <t>04/12/2025</t>
+          <t>26/11/2025</t>
         </is>
       </c>
       <c r="F9" s="8" t="inlineStr">
         <is>
-          <t>14:00:00</t>
+          <t>12:00:00</t>
         </is>
       </c>
       <c r="G9" s="9" t="n">
@@ -810,22 +810,22 @@
       </c>
       <c r="C10" s="2" t="inlineStr">
         <is>
-          <t>pharmacology</t>
+          <t>microbiology</t>
         </is>
       </c>
       <c r="D10" s="2" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>2</t>
         </is>
       </c>
       <c r="E10" s="3" t="inlineStr">
         <is>
-          <t>30/11/2025</t>
+          <t>08/12/2025</t>
         </is>
       </c>
       <c r="F10" s="4" t="inlineStr">
         <is>
-          <t>08:00:00</t>
+          <t>14:00:00</t>
         </is>
       </c>
       <c r="G10" s="5" t="n">
@@ -845,22 +845,22 @@
       </c>
       <c r="C11" s="6" t="inlineStr">
         <is>
-          <t>pharmacology</t>
+          <t>parasitology sgd/pos</t>
         </is>
       </c>
       <c r="D11" s="6" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>1</t>
         </is>
       </c>
       <c r="E11" s="7" t="inlineStr">
         <is>
-          <t>09/12/2025</t>
+          <t>11/12/2025</t>
         </is>
       </c>
       <c r="F11" s="8" t="inlineStr">
         <is>
-          <t>10:00:00</t>
+          <t>14:00:00</t>
         </is>
       </c>
       <c r="G11" s="9" t="n">
@@ -880,7 +880,7 @@
       </c>
       <c r="C12" s="2" t="inlineStr">
         <is>
-          <t>physiology</t>
+          <t>pathology lab/museum</t>
         </is>
       </c>
       <c r="D12" s="2" t="inlineStr">
@@ -890,16 +890,16 @@
       </c>
       <c r="E12" s="3" t="inlineStr">
         <is>
-          <t>12/11/2025</t>
+          <t>04/12/2025</t>
         </is>
       </c>
       <c r="F12" s="4" t="inlineStr">
         <is>
-          <t>12:00:00</t>
+          <t>14:00:00</t>
         </is>
       </c>
       <c r="G12" s="5" t="n">
-        <v>90</v>
+        <v>120</v>
       </c>
     </row>
     <row r="13">
@@ -915,7 +915,7 @@
       </c>
       <c r="C13" s="6" t="inlineStr">
         <is>
-          <t>physiology</t>
+          <t>pathology lab/museum</t>
         </is>
       </c>
       <c r="D13" s="6" t="inlineStr">
@@ -925,16 +925,16 @@
       </c>
       <c r="E13" s="7" t="inlineStr">
         <is>
-          <t>19/11/2025</t>
+          <t>07/12/2025</t>
         </is>
       </c>
       <c r="F13" s="8" t="inlineStr">
         <is>
-          <t>15:00:00</t>
+          <t>08:00:00</t>
         </is>
       </c>
       <c r="G13" s="9" t="n">
-        <v>90</v>
+        <v>120</v>
       </c>
     </row>
     <row r="14">
@@ -950,7 +950,7 @@
       </c>
       <c r="C14" s="2" t="inlineStr">
         <is>
-          <t>physiology</t>
+          <t>pathology lab/museum</t>
         </is>
       </c>
       <c r="D14" s="2" t="inlineStr">
@@ -960,16 +960,16 @@
       </c>
       <c r="E14" s="3" t="inlineStr">
         <is>
-          <t>20/11/2025</t>
+          <t>16/12/2025</t>
         </is>
       </c>
       <c r="F14" s="4" t="inlineStr">
         <is>
-          <t>12:00:00</t>
+          <t>14:00:00</t>
         </is>
       </c>
       <c r="G14" s="5" t="n">
-        <v>90</v>
+        <v>120</v>
       </c>
     </row>
     <row r="15">
@@ -980,31 +980,31 @@
       </c>
       <c r="B15" s="6" t="inlineStr">
         <is>
-          <t>A2</t>
+          <t>A1</t>
         </is>
       </c>
       <c r="C15" s="6" t="inlineStr">
         <is>
-          <t>anatomy</t>
+          <t>pathology lab/museum</t>
         </is>
       </c>
       <c r="D15" s="6" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>4</t>
         </is>
       </c>
       <c r="E15" s="7" t="inlineStr">
         <is>
-          <t>11/11/2025</t>
+          <t>16/12/2025</t>
         </is>
       </c>
       <c r="F15" s="8" t="inlineStr">
         <is>
-          <t>09:00:00</t>
+          <t>12:00:00</t>
         </is>
       </c>
       <c r="G15" s="9" t="n">
-        <v>90</v>
+        <v>120</v>
       </c>
     </row>
     <row r="16">
@@ -1015,12 +1015,12 @@
       </c>
       <c r="B16" s="2" t="inlineStr">
         <is>
-          <t>A2</t>
+          <t>A1</t>
         </is>
       </c>
       <c r="C16" s="2" t="inlineStr">
         <is>
-          <t>biochemistry lab/cbl</t>
+          <t>pharmacology</t>
         </is>
       </c>
       <c r="D16" s="2" t="inlineStr">
@@ -1030,12 +1030,12 @@
       </c>
       <c r="E16" s="3" t="inlineStr">
         <is>
-          <t>24/11/2025</t>
+          <t>30/11/2025</t>
         </is>
       </c>
       <c r="F16" s="4" t="inlineStr">
         <is>
-          <t>12:00:00</t>
+          <t>08:00:00</t>
         </is>
       </c>
       <c r="G16" s="5" t="n">
@@ -1050,27 +1050,27 @@
       </c>
       <c r="B17" s="6" t="inlineStr">
         <is>
-          <t>A2</t>
+          <t>A1</t>
         </is>
       </c>
       <c r="C17" s="6" t="inlineStr">
         <is>
-          <t>histology</t>
+          <t>pharmacology</t>
         </is>
       </c>
       <c r="D17" s="6" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>2</t>
         </is>
       </c>
       <c r="E17" s="7" t="inlineStr">
         <is>
-          <t>13/11/2025</t>
+          <t>09/12/2025</t>
         </is>
       </c>
       <c r="F17" s="8" t="inlineStr">
         <is>
-          <t>14:00:00</t>
+          <t>10:00:00</t>
         </is>
       </c>
       <c r="G17" s="9" t="n">
@@ -1085,31 +1085,31 @@
       </c>
       <c r="B18" s="2" t="inlineStr">
         <is>
-          <t>A2</t>
+          <t>A1</t>
         </is>
       </c>
       <c r="C18" s="2" t="inlineStr">
         <is>
-          <t>histology</t>
+          <t>physiology</t>
         </is>
       </c>
       <c r="D18" s="2" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>1</t>
         </is>
       </c>
       <c r="E18" s="3" t="inlineStr">
         <is>
-          <t>04/12/2025</t>
+          <t>12/11/2025</t>
         </is>
       </c>
       <c r="F18" s="4" t="inlineStr">
         <is>
-          <t>14:00:00</t>
+          <t>12:00:00</t>
         </is>
       </c>
       <c r="G18" s="5" t="n">
-        <v>120</v>
+        <v>90</v>
       </c>
     </row>
     <row r="19">
@@ -1120,31 +1120,31 @@
       </c>
       <c r="B19" s="6" t="inlineStr">
         <is>
-          <t>A2</t>
+          <t>A1</t>
         </is>
       </c>
       <c r="C19" s="6" t="inlineStr">
         <is>
-          <t>histology</t>
+          <t>physiology</t>
         </is>
       </c>
       <c r="D19" s="6" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>2</t>
         </is>
       </c>
       <c r="E19" s="7" t="inlineStr">
         <is>
-          <t>11/12/2025</t>
+          <t>19/11/2025</t>
         </is>
       </c>
       <c r="F19" s="8" t="inlineStr">
         <is>
-          <t>08:00:00</t>
+          <t>15:00:00</t>
         </is>
       </c>
       <c r="G19" s="9" t="n">
-        <v>120</v>
+        <v>90</v>
       </c>
     </row>
     <row r="20">
@@ -1155,31 +1155,31 @@
       </c>
       <c r="B20" s="2" t="inlineStr">
         <is>
-          <t>A2</t>
+          <t>A1</t>
         </is>
       </c>
       <c r="C20" s="2" t="inlineStr">
         <is>
-          <t>microbiology</t>
+          <t>physiology</t>
         </is>
       </c>
       <c r="D20" s="2" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>3</t>
         </is>
       </c>
       <c r="E20" s="3" t="inlineStr">
         <is>
-          <t>23/11/2025</t>
+          <t>20/11/2025</t>
         </is>
       </c>
       <c r="F20" s="4" t="inlineStr">
         <is>
-          <t>10:00:00</t>
+          <t>12:00:00</t>
         </is>
       </c>
       <c r="G20" s="5" t="n">
-        <v>120</v>
+        <v>90</v>
       </c>
     </row>
     <row r="21">
@@ -1195,26 +1195,26 @@
       </c>
       <c r="C21" s="6" t="inlineStr">
         <is>
-          <t>microbiology</t>
+          <t>anatomy</t>
         </is>
       </c>
       <c r="D21" s="6" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>1</t>
         </is>
       </c>
       <c r="E21" s="7" t="inlineStr">
         <is>
-          <t>10/12/2025</t>
+          <t>11/11/2025</t>
         </is>
       </c>
       <c r="F21" s="8" t="inlineStr">
         <is>
-          <t>12:00:00</t>
+          <t>09:00:00</t>
         </is>
       </c>
       <c r="G21" s="9" t="n">
-        <v>120</v>
+        <v>90</v>
       </c>
     </row>
     <row r="22">
@@ -1230,22 +1230,22 @@
       </c>
       <c r="C22" s="2" t="inlineStr">
         <is>
-          <t>parasitology sgd/pos</t>
+          <t>anatomy</t>
         </is>
       </c>
       <c r="D22" s="2" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>2</t>
         </is>
       </c>
       <c r="E22" s="3" t="inlineStr">
         <is>
-          <t>11/12/2025</t>
+          <t>09/12/2025</t>
         </is>
       </c>
       <c r="F22" s="4" t="inlineStr">
         <is>
-          <t>12:00:00</t>
+          <t>10:00:00</t>
         </is>
       </c>
       <c r="G22" s="5" t="n">
@@ -1265,22 +1265,22 @@
       </c>
       <c r="C23" s="6" t="inlineStr">
         <is>
-          <t>pathology lab/museum</t>
+          <t>anatomy</t>
         </is>
       </c>
       <c r="D23" s="6" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>3</t>
         </is>
       </c>
       <c r="E23" s="7" t="inlineStr">
         <is>
-          <t>04/12/2025</t>
+          <t>15/12/2025</t>
         </is>
       </c>
       <c r="F23" s="8" t="inlineStr">
         <is>
-          <t>12:00:00</t>
+          <t>14:00:00</t>
         </is>
       </c>
       <c r="G23" s="9" t="n">
@@ -1300,7 +1300,7 @@
       </c>
       <c r="C24" s="2" t="inlineStr">
         <is>
-          <t>pharmacology</t>
+          <t>biochemistry lab/cbl</t>
         </is>
       </c>
       <c r="D24" s="2" t="inlineStr">
@@ -1310,12 +1310,12 @@
       </c>
       <c r="E24" s="3" t="inlineStr">
         <is>
-          <t>30/11/2025</t>
+          <t>24/11/2025</t>
         </is>
       </c>
       <c r="F24" s="4" t="inlineStr">
         <is>
-          <t>10:00:00</t>
+          <t>12:00:00</t>
         </is>
       </c>
       <c r="G24" s="5" t="n">
@@ -1335,22 +1335,22 @@
       </c>
       <c r="C25" s="6" t="inlineStr">
         <is>
-          <t>pharmacology</t>
+          <t>histology</t>
         </is>
       </c>
       <c r="D25" s="6" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>1</t>
         </is>
       </c>
       <c r="E25" s="7" t="inlineStr">
         <is>
-          <t>09/12/2025</t>
+          <t>13/11/2025</t>
         </is>
       </c>
       <c r="F25" s="8" t="inlineStr">
         <is>
-          <t>08:00:00</t>
+          <t>14:00:00</t>
         </is>
       </c>
       <c r="G25" s="9" t="n">
@@ -1370,26 +1370,26 @@
       </c>
       <c r="C26" s="2" t="inlineStr">
         <is>
-          <t>physiology</t>
+          <t>histology</t>
         </is>
       </c>
       <c r="D26" s="2" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>2</t>
         </is>
       </c>
       <c r="E26" s="3" t="inlineStr">
         <is>
-          <t>12/11/2025</t>
+          <t>04/12/2025</t>
         </is>
       </c>
       <c r="F26" s="4" t="inlineStr">
         <is>
-          <t>13:00:00</t>
+          <t>14:00:00</t>
         </is>
       </c>
       <c r="G26" s="5" t="n">
-        <v>90</v>
+        <v>120</v>
       </c>
     </row>
     <row r="27">
@@ -1405,26 +1405,26 @@
       </c>
       <c r="C27" s="6" t="inlineStr">
         <is>
-          <t>physiology</t>
+          <t>histology</t>
         </is>
       </c>
       <c r="D27" s="6" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>3</t>
         </is>
       </c>
       <c r="E27" s="7" t="inlineStr">
         <is>
-          <t>20/11/2025</t>
+          <t>11/12/2025</t>
         </is>
       </c>
       <c r="F27" s="8" t="inlineStr">
         <is>
-          <t>09:00:00</t>
+          <t>08:00:00</t>
         </is>
       </c>
       <c r="G27" s="9" t="n">
-        <v>90</v>
+        <v>120</v>
       </c>
     </row>
     <row r="28">
@@ -1440,26 +1440,26 @@
       </c>
       <c r="C28" s="2" t="inlineStr">
         <is>
-          <t>physiology</t>
+          <t>microbiology</t>
         </is>
       </c>
       <c r="D28" s="2" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>1</t>
         </is>
       </c>
       <c r="E28" s="3" t="inlineStr">
         <is>
-          <t>20/11/2025</t>
+          <t>23/11/2025</t>
         </is>
       </c>
       <c r="F28" s="4" t="inlineStr">
         <is>
-          <t>15:00:00</t>
+          <t>10:00:00</t>
         </is>
       </c>
       <c r="G28" s="5" t="n">
-        <v>90</v>
+        <v>120</v>
       </c>
     </row>
     <row r="29">
@@ -1470,31 +1470,31 @@
       </c>
       <c r="B29" s="6" t="inlineStr">
         <is>
-          <t>A3</t>
+          <t>A2</t>
         </is>
       </c>
       <c r="C29" s="6" t="inlineStr">
         <is>
-          <t>anatomy</t>
+          <t>microbiology</t>
         </is>
       </c>
       <c r="D29" s="6" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>2</t>
         </is>
       </c>
       <c r="E29" s="7" t="inlineStr">
         <is>
-          <t>11/11/2025</t>
+          <t>10/12/2025</t>
         </is>
       </c>
       <c r="F29" s="8" t="inlineStr">
         <is>
-          <t>10:00:00</t>
+          <t>12:00:00</t>
         </is>
       </c>
       <c r="G29" s="9" t="n">
-        <v>90</v>
+        <v>120</v>
       </c>
     </row>
     <row r="30">
@@ -1505,12 +1505,12 @@
       </c>
       <c r="B30" s="2" t="inlineStr">
         <is>
-          <t>A3</t>
+          <t>A2</t>
         </is>
       </c>
       <c r="C30" s="2" t="inlineStr">
         <is>
-          <t>biochemistry lab/cbl</t>
+          <t>parasitology sgd/pos</t>
         </is>
       </c>
       <c r="D30" s="2" t="inlineStr">
@@ -1520,12 +1520,12 @@
       </c>
       <c r="E30" s="3" t="inlineStr">
         <is>
-          <t>19/11/2025</t>
+          <t>11/12/2025</t>
         </is>
       </c>
       <c r="F30" s="4" t="inlineStr">
         <is>
-          <t>14:00:00</t>
+          <t>12:00:00</t>
         </is>
       </c>
       <c r="G30" s="5" t="n">
@@ -1540,12 +1540,12 @@
       </c>
       <c r="B31" s="6" t="inlineStr">
         <is>
-          <t>A3</t>
+          <t>A2</t>
         </is>
       </c>
       <c r="C31" s="6" t="inlineStr">
         <is>
-          <t>histology</t>
+          <t>pathology lab/museum</t>
         </is>
       </c>
       <c r="D31" s="6" t="inlineStr">
@@ -1555,12 +1555,12 @@
       </c>
       <c r="E31" s="7" t="inlineStr">
         <is>
-          <t>11/11/2025</t>
+          <t>04/12/2025</t>
         </is>
       </c>
       <c r="F31" s="8" t="inlineStr">
         <is>
-          <t>08:00:00</t>
+          <t>12:00:00</t>
         </is>
       </c>
       <c r="G31" s="9" t="n">
@@ -1575,12 +1575,12 @@
       </c>
       <c r="B32" s="2" t="inlineStr">
         <is>
-          <t>A3</t>
+          <t>A2</t>
         </is>
       </c>
       <c r="C32" s="2" t="inlineStr">
         <is>
-          <t>histology</t>
+          <t>pathology lab/museum</t>
         </is>
       </c>
       <c r="D32" s="2" t="inlineStr">
@@ -1590,12 +1590,12 @@
       </c>
       <c r="E32" s="3" t="inlineStr">
         <is>
-          <t>04/12/2025</t>
+          <t>08/12/2025</t>
         </is>
       </c>
       <c r="F32" s="4" t="inlineStr">
         <is>
-          <t>10:00:00</t>
+          <t>14:00:00</t>
         </is>
       </c>
       <c r="G32" s="5" t="n">
@@ -1610,27 +1610,27 @@
       </c>
       <c r="B33" s="6" t="inlineStr">
         <is>
-          <t>A3</t>
+          <t>A2</t>
         </is>
       </c>
       <c r="C33" s="6" t="inlineStr">
         <is>
-          <t>microbiology</t>
+          <t>pathology lab/museum</t>
         </is>
       </c>
       <c r="D33" s="6" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>3</t>
         </is>
       </c>
       <c r="E33" s="7" t="inlineStr">
         <is>
-          <t>25/11/2025</t>
+          <t>17/12/2025</t>
         </is>
       </c>
       <c r="F33" s="8" t="inlineStr">
         <is>
-          <t>08:00:00</t>
+          <t>14:00:00</t>
         </is>
       </c>
       <c r="G33" s="9" t="n">
@@ -1645,27 +1645,27 @@
       </c>
       <c r="B34" s="2" t="inlineStr">
         <is>
-          <t>A3</t>
+          <t>A2</t>
         </is>
       </c>
       <c r="C34" s="2" t="inlineStr">
         <is>
-          <t>microbiology</t>
+          <t>pathology lab/museum</t>
         </is>
       </c>
       <c r="D34" s="2" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>4</t>
         </is>
       </c>
       <c r="E34" s="3" t="inlineStr">
         <is>
-          <t>09/12/2025</t>
+          <t>16/12/2025</t>
         </is>
       </c>
       <c r="F34" s="4" t="inlineStr">
         <is>
-          <t>08:00:00</t>
+          <t>14:00:00</t>
         </is>
       </c>
       <c r="G34" s="5" t="n">
@@ -1680,12 +1680,12 @@
       </c>
       <c r="B35" s="6" t="inlineStr">
         <is>
-          <t>A3</t>
+          <t>A2</t>
         </is>
       </c>
       <c r="C35" s="6" t="inlineStr">
         <is>
-          <t>parasitology sgd/pos</t>
+          <t>pharmacology</t>
         </is>
       </c>
       <c r="D35" s="6" t="inlineStr">
@@ -1695,7 +1695,7 @@
       </c>
       <c r="E35" s="7" t="inlineStr">
         <is>
-          <t>09/12/2025</t>
+          <t>30/11/2025</t>
         </is>
       </c>
       <c r="F35" s="8" t="inlineStr">
@@ -1715,22 +1715,22 @@
       </c>
       <c r="B36" s="2" t="inlineStr">
         <is>
-          <t>A3</t>
+          <t>A2</t>
         </is>
       </c>
       <c r="C36" s="2" t="inlineStr">
         <is>
-          <t>pathology lab/museum</t>
+          <t>pharmacology</t>
         </is>
       </c>
       <c r="D36" s="2" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>2</t>
         </is>
       </c>
       <c r="E36" s="3" t="inlineStr">
         <is>
-          <t>04/12/2025</t>
+          <t>09/12/2025</t>
         </is>
       </c>
       <c r="F36" s="4" t="inlineStr">
@@ -1750,12 +1750,12 @@
       </c>
       <c r="B37" s="6" t="inlineStr">
         <is>
-          <t>A3</t>
+          <t>A2</t>
         </is>
       </c>
       <c r="C37" s="6" t="inlineStr">
         <is>
-          <t>pharmacology</t>
+          <t>physiology</t>
         </is>
       </c>
       <c r="D37" s="6" t="inlineStr">
@@ -1765,16 +1765,16 @@
       </c>
       <c r="E37" s="7" t="inlineStr">
         <is>
-          <t>02/12/2025</t>
+          <t>12/11/2025</t>
         </is>
       </c>
       <c r="F37" s="8" t="inlineStr">
         <is>
-          <t>10:00:00</t>
+          <t>13:00:00</t>
         </is>
       </c>
       <c r="G37" s="9" t="n">
-        <v>120</v>
+        <v>90</v>
       </c>
     </row>
     <row r="38">
@@ -1785,12 +1785,12 @@
       </c>
       <c r="B38" s="2" t="inlineStr">
         <is>
-          <t>A3</t>
+          <t>A2</t>
         </is>
       </c>
       <c r="C38" s="2" t="inlineStr">
         <is>
-          <t>pharmacology</t>
+          <t>physiology</t>
         </is>
       </c>
       <c r="D38" s="2" t="inlineStr">
@@ -1800,16 +1800,16 @@
       </c>
       <c r="E38" s="3" t="inlineStr">
         <is>
-          <t>11/12/2025</t>
+          <t>20/11/2025</t>
         </is>
       </c>
       <c r="F38" s="4" t="inlineStr">
         <is>
-          <t>12:00:00</t>
+          <t>09:00:00</t>
         </is>
       </c>
       <c r="G38" s="5" t="n">
-        <v>120</v>
+        <v>90</v>
       </c>
     </row>
     <row r="39">
@@ -1820,7 +1820,7 @@
       </c>
       <c r="B39" s="6" t="inlineStr">
         <is>
-          <t>A3</t>
+          <t>A2</t>
         </is>
       </c>
       <c r="C39" s="6" t="inlineStr">
@@ -1830,17 +1830,17 @@
       </c>
       <c r="D39" s="6" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>3</t>
         </is>
       </c>
       <c r="E39" s="7" t="inlineStr">
         <is>
-          <t>12/11/2025</t>
+          <t>20/11/2025</t>
         </is>
       </c>
       <c r="F39" s="8" t="inlineStr">
         <is>
-          <t>14:00:00</t>
+          <t>15:00:00</t>
         </is>
       </c>
       <c r="G39" s="9" t="n">
@@ -1860,22 +1860,22 @@
       </c>
       <c r="C40" s="2" t="inlineStr">
         <is>
-          <t>physiology</t>
+          <t>anatomy</t>
         </is>
       </c>
       <c r="D40" s="2" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>1</t>
         </is>
       </c>
       <c r="E40" s="3" t="inlineStr">
         <is>
-          <t>20/11/2025</t>
+          <t>11/11/2025</t>
         </is>
       </c>
       <c r="F40" s="4" t="inlineStr">
         <is>
-          <t>08:00:00</t>
+          <t>10:00:00</t>
         </is>
       </c>
       <c r="G40" s="5" t="n">
@@ -1895,26 +1895,26 @@
       </c>
       <c r="C41" s="6" t="inlineStr">
         <is>
-          <t>physiology</t>
+          <t>anatomy</t>
         </is>
       </c>
       <c r="D41" s="6" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>2</t>
         </is>
       </c>
       <c r="E41" s="7" t="inlineStr">
         <is>
-          <t>20/11/2025</t>
+          <t>11/12/2025</t>
         </is>
       </c>
       <c r="F41" s="8" t="inlineStr">
         <is>
-          <t>13:00:00</t>
+          <t>10:00:00</t>
         </is>
       </c>
       <c r="G41" s="9" t="n">
-        <v>90</v>
+        <v>120</v>
       </c>
     </row>
     <row r="42">
@@ -1925,7 +1925,7 @@
       </c>
       <c r="B42" s="2" t="inlineStr">
         <is>
-          <t>B1</t>
+          <t>A3</t>
         </is>
       </c>
       <c r="C42" s="2" t="inlineStr">
@@ -1935,21 +1935,21 @@
       </c>
       <c r="D42" s="2" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>3</t>
         </is>
       </c>
       <c r="E42" s="3" t="inlineStr">
         <is>
-          <t>13/11/2025</t>
+          <t>16/12/2025</t>
         </is>
       </c>
       <c r="F42" s="4" t="inlineStr">
         <is>
-          <t>12:00:00</t>
+          <t>10:00:00</t>
         </is>
       </c>
       <c r="G42" s="5" t="n">
-        <v>90</v>
+        <v>120</v>
       </c>
     </row>
     <row r="43">
@@ -1960,7 +1960,7 @@
       </c>
       <c r="B43" s="6" t="inlineStr">
         <is>
-          <t>B1</t>
+          <t>A3</t>
         </is>
       </c>
       <c r="C43" s="6" t="inlineStr">
@@ -1975,7 +1975,7 @@
       </c>
       <c r="E43" s="7" t="inlineStr">
         <is>
-          <t>13/11/2025</t>
+          <t>19/11/2025</t>
         </is>
       </c>
       <c r="F43" s="8" t="inlineStr">
@@ -1995,7 +1995,7 @@
       </c>
       <c r="B44" s="2" t="inlineStr">
         <is>
-          <t>B1</t>
+          <t>A3</t>
         </is>
       </c>
       <c r="C44" s="2" t="inlineStr">
@@ -2010,12 +2010,12 @@
       </c>
       <c r="E44" s="3" t="inlineStr">
         <is>
-          <t>10/11/2025</t>
+          <t>11/11/2025</t>
         </is>
       </c>
       <c r="F44" s="4" t="inlineStr">
         <is>
-          <t>14:00:00</t>
+          <t>08:00:00</t>
         </is>
       </c>
       <c r="G44" s="5" t="n">
@@ -2030,7 +2030,7 @@
       </c>
       <c r="B45" s="6" t="inlineStr">
         <is>
-          <t>B1</t>
+          <t>A3</t>
         </is>
       </c>
       <c r="C45" s="6" t="inlineStr">
@@ -2045,12 +2045,12 @@
       </c>
       <c r="E45" s="7" t="inlineStr">
         <is>
-          <t>03/12/2025</t>
+          <t>04/12/2025</t>
         </is>
       </c>
       <c r="F45" s="8" t="inlineStr">
         <is>
-          <t>14:00:00</t>
+          <t>10:00:00</t>
         </is>
       </c>
       <c r="G45" s="9" t="n">
@@ -2065,7 +2065,7 @@
       </c>
       <c r="B46" s="2" t="inlineStr">
         <is>
-          <t>B1</t>
+          <t>A3</t>
         </is>
       </c>
       <c r="C46" s="2" t="inlineStr">
@@ -2080,12 +2080,12 @@
       </c>
       <c r="E46" s="3" t="inlineStr">
         <is>
-          <t>11/12/2025</t>
+          <t>14/12/2025</t>
         </is>
       </c>
       <c r="F46" s="4" t="inlineStr">
         <is>
-          <t>10:00:00</t>
+          <t>08:00:00</t>
         </is>
       </c>
       <c r="G46" s="5" t="n">
@@ -2100,7 +2100,7 @@
       </c>
       <c r="B47" s="6" t="inlineStr">
         <is>
-          <t>B1</t>
+          <t>A3</t>
         </is>
       </c>
       <c r="C47" s="6" t="inlineStr">
@@ -2115,12 +2115,12 @@
       </c>
       <c r="E47" s="7" t="inlineStr">
         <is>
-          <t>24/11/2025</t>
+          <t>25/11/2025</t>
         </is>
       </c>
       <c r="F47" s="8" t="inlineStr">
         <is>
-          <t>14:00:00</t>
+          <t>08:00:00</t>
         </is>
       </c>
       <c r="G47" s="9" t="n">
@@ -2135,7 +2135,7 @@
       </c>
       <c r="B48" s="2" t="inlineStr">
         <is>
-          <t>B1</t>
+          <t>A3</t>
         </is>
       </c>
       <c r="C48" s="2" t="inlineStr">
@@ -2150,12 +2150,12 @@
       </c>
       <c r="E48" s="3" t="inlineStr">
         <is>
-          <t>10/12/2025</t>
+          <t>09/12/2025</t>
         </is>
       </c>
       <c r="F48" s="4" t="inlineStr">
         <is>
-          <t>14:00:00</t>
+          <t>08:00:00</t>
         </is>
       </c>
       <c r="G48" s="5" t="n">
@@ -2170,7 +2170,7 @@
       </c>
       <c r="B49" s="6" t="inlineStr">
         <is>
-          <t>B1</t>
+          <t>A3</t>
         </is>
       </c>
       <c r="C49" s="6" t="inlineStr">
@@ -2185,12 +2185,12 @@
       </c>
       <c r="E49" s="7" t="inlineStr">
         <is>
-          <t>10/12/2025</t>
+          <t>09/12/2025</t>
         </is>
       </c>
       <c r="F49" s="8" t="inlineStr">
         <is>
-          <t>12:00:00</t>
+          <t>10:00:00</t>
         </is>
       </c>
       <c r="G49" s="9" t="n">
@@ -2205,7 +2205,7 @@
       </c>
       <c r="B50" s="2" t="inlineStr">
         <is>
-          <t>B1</t>
+          <t>A3</t>
         </is>
       </c>
       <c r="C50" s="2" t="inlineStr">
@@ -2220,12 +2220,12 @@
       </c>
       <c r="E50" s="3" t="inlineStr">
         <is>
-          <t>03/12/2025</t>
+          <t>04/12/2025</t>
         </is>
       </c>
       <c r="F50" s="4" t="inlineStr">
         <is>
-          <t>14:00:00</t>
+          <t>08:00:00</t>
         </is>
       </c>
       <c r="G50" s="5" t="n">
@@ -2240,27 +2240,27 @@
       </c>
       <c r="B51" s="6" t="inlineStr">
         <is>
-          <t>B1</t>
+          <t>A3</t>
         </is>
       </c>
       <c r="C51" s="6" t="inlineStr">
         <is>
-          <t>pharmacology</t>
+          <t>pathology lab/museum</t>
         </is>
       </c>
       <c r="D51" s="6" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>2</t>
         </is>
       </c>
       <c r="E51" s="7" t="inlineStr">
         <is>
-          <t>01/12/2025</t>
+          <t>08/12/2025</t>
         </is>
       </c>
       <c r="F51" s="8" t="inlineStr">
         <is>
-          <t>14:00:00</t>
+          <t>12:00:00</t>
         </is>
       </c>
       <c r="G51" s="9" t="n">
@@ -2275,27 +2275,27 @@
       </c>
       <c r="B52" s="2" t="inlineStr">
         <is>
-          <t>B1</t>
+          <t>A3</t>
         </is>
       </c>
       <c r="C52" s="2" t="inlineStr">
         <is>
-          <t>pharmacology</t>
+          <t>pathology lab/museum</t>
         </is>
       </c>
       <c r="D52" s="2" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>3</t>
         </is>
       </c>
       <c r="E52" s="3" t="inlineStr">
         <is>
-          <t>08/12/2025</t>
+          <t>16/12/2025</t>
         </is>
       </c>
       <c r="F52" s="4" t="inlineStr">
         <is>
-          <t>14:00:00</t>
+          <t>12:00:00</t>
         </is>
       </c>
       <c r="G52" s="5" t="n">
@@ -2310,31 +2310,31 @@
       </c>
       <c r="B53" s="6" t="inlineStr">
         <is>
-          <t>B1</t>
+          <t>A3</t>
         </is>
       </c>
       <c r="C53" s="6" t="inlineStr">
         <is>
-          <t>physiology</t>
+          <t>pathology lab/museum</t>
         </is>
       </c>
       <c r="D53" s="6" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>4</t>
         </is>
       </c>
       <c r="E53" s="7" t="inlineStr">
         <is>
-          <t>12/11/2025</t>
+          <t>17/12/2025</t>
         </is>
       </c>
       <c r="F53" s="8" t="inlineStr">
         <is>
-          <t>13:00:00</t>
+          <t>12:00:00</t>
         </is>
       </c>
       <c r="G53" s="9" t="n">
-        <v>90</v>
+        <v>120</v>
       </c>
     </row>
     <row r="54">
@@ -2345,31 +2345,31 @@
       </c>
       <c r="B54" s="2" t="inlineStr">
         <is>
-          <t>B1</t>
+          <t>A3</t>
         </is>
       </c>
       <c r="C54" s="2" t="inlineStr">
         <is>
-          <t>physiology</t>
+          <t>pharmacology</t>
         </is>
       </c>
       <c r="D54" s="2" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>1</t>
         </is>
       </c>
       <c r="E54" s="3" t="inlineStr">
         <is>
-          <t>19/11/2025</t>
+          <t>02/12/2025</t>
         </is>
       </c>
       <c r="F54" s="4" t="inlineStr">
         <is>
-          <t>12:00:00</t>
+          <t>10:00:00</t>
         </is>
       </c>
       <c r="G54" s="5" t="n">
-        <v>90</v>
+        <v>120</v>
       </c>
     </row>
     <row r="55">
@@ -2380,31 +2380,31 @@
       </c>
       <c r="B55" s="6" t="inlineStr">
         <is>
-          <t>B1</t>
+          <t>A3</t>
         </is>
       </c>
       <c r="C55" s="6" t="inlineStr">
         <is>
-          <t>physiology</t>
+          <t>pharmacology</t>
         </is>
       </c>
       <c r="D55" s="6" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>2</t>
         </is>
       </c>
       <c r="E55" s="7" t="inlineStr">
         <is>
-          <t>20/11/2025</t>
+          <t>11/12/2025</t>
         </is>
       </c>
       <c r="F55" s="8" t="inlineStr">
         <is>
-          <t>11:00:00</t>
+          <t>12:00:00</t>
         </is>
       </c>
       <c r="G55" s="9" t="n">
-        <v>90</v>
+        <v>120</v>
       </c>
     </row>
     <row r="56">
@@ -2415,12 +2415,12 @@
       </c>
       <c r="B56" s="2" t="inlineStr">
         <is>
-          <t>B2</t>
+          <t>A3</t>
         </is>
       </c>
       <c r="C56" s="2" t="inlineStr">
         <is>
-          <t>anatomy</t>
+          <t>physiology</t>
         </is>
       </c>
       <c r="D56" s="2" t="inlineStr">
@@ -2430,7 +2430,7 @@
       </c>
       <c r="E56" s="3" t="inlineStr">
         <is>
-          <t>13/11/2025</t>
+          <t>12/11/2025</t>
         </is>
       </c>
       <c r="F56" s="4" t="inlineStr">
@@ -2450,31 +2450,31 @@
       </c>
       <c r="B57" s="6" t="inlineStr">
         <is>
-          <t>B2</t>
+          <t>A3</t>
         </is>
       </c>
       <c r="C57" s="6" t="inlineStr">
         <is>
-          <t>biochemistry lab/cbl</t>
+          <t>physiology</t>
         </is>
       </c>
       <c r="D57" s="6" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>2</t>
         </is>
       </c>
       <c r="E57" s="7" t="inlineStr">
         <is>
-          <t>24/11/2025</t>
+          <t>20/11/2025</t>
         </is>
       </c>
       <c r="F57" s="8" t="inlineStr">
         <is>
-          <t>14:00:00</t>
+          <t>08:00:00</t>
         </is>
       </c>
       <c r="G57" s="9" t="n">
-        <v>120</v>
+        <v>90</v>
       </c>
     </row>
     <row r="58">
@@ -2485,31 +2485,31 @@
       </c>
       <c r="B58" s="2" t="inlineStr">
         <is>
-          <t>B2</t>
+          <t>A3</t>
         </is>
       </c>
       <c r="C58" s="2" t="inlineStr">
         <is>
-          <t>histology</t>
+          <t>physiology</t>
         </is>
       </c>
       <c r="D58" s="2" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>3</t>
         </is>
       </c>
       <c r="E58" s="3" t="inlineStr">
         <is>
-          <t>13/11/2025</t>
+          <t>20/11/2025</t>
         </is>
       </c>
       <c r="F58" s="4" t="inlineStr">
         <is>
-          <t>12:00:00</t>
+          <t>13:00:00</t>
         </is>
       </c>
       <c r="G58" s="5" t="n">
-        <v>120</v>
+        <v>90</v>
       </c>
     </row>
     <row r="59">
@@ -2520,31 +2520,31 @@
       </c>
       <c r="B59" s="6" t="inlineStr">
         <is>
-          <t>B2</t>
+          <t>B1</t>
         </is>
       </c>
       <c r="C59" s="6" t="inlineStr">
         <is>
-          <t>histology</t>
+          <t>anatomy</t>
         </is>
       </c>
       <c r="D59" s="6" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>1</t>
         </is>
       </c>
       <c r="E59" s="7" t="inlineStr">
         <is>
-          <t>01/12/2025</t>
+          <t>13/11/2025</t>
         </is>
       </c>
       <c r="F59" s="8" t="inlineStr">
         <is>
-          <t>14:00:00</t>
+          <t>12:00:00</t>
         </is>
       </c>
       <c r="G59" s="9" t="n">
-        <v>120</v>
+        <v>90</v>
       </c>
     </row>
     <row r="60">
@@ -2555,17 +2555,17 @@
       </c>
       <c r="B60" s="2" t="inlineStr">
         <is>
-          <t>B2</t>
+          <t>B1</t>
         </is>
       </c>
       <c r="C60" s="2" t="inlineStr">
         <is>
-          <t>histology</t>
+          <t>anatomy</t>
         </is>
       </c>
       <c r="D60" s="2" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>2</t>
         </is>
       </c>
       <c r="E60" s="3" t="inlineStr">
@@ -2590,27 +2590,27 @@
       </c>
       <c r="B61" s="6" t="inlineStr">
         <is>
-          <t>B2</t>
+          <t>B1</t>
         </is>
       </c>
       <c r="C61" s="6" t="inlineStr">
         <is>
-          <t>microbiology</t>
+          <t>anatomy</t>
         </is>
       </c>
       <c r="D61" s="6" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>3</t>
         </is>
       </c>
       <c r="E61" s="7" t="inlineStr">
         <is>
-          <t>24/11/2025</t>
+          <t>17/12/2025</t>
         </is>
       </c>
       <c r="F61" s="8" t="inlineStr">
         <is>
-          <t>12:00:00</t>
+          <t>08:00:00</t>
         </is>
       </c>
       <c r="G61" s="9" t="n">
@@ -2625,27 +2625,27 @@
       </c>
       <c r="B62" s="2" t="inlineStr">
         <is>
-          <t>B2</t>
+          <t>B1</t>
         </is>
       </c>
       <c r="C62" s="2" t="inlineStr">
         <is>
-          <t>microbiology</t>
+          <t>biochemistry lab/cbl</t>
         </is>
       </c>
       <c r="D62" s="2" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>1</t>
         </is>
       </c>
       <c r="E62" s="3" t="inlineStr">
         <is>
-          <t>09/12/2025</t>
+          <t>13/11/2025</t>
         </is>
       </c>
       <c r="F62" s="4" t="inlineStr">
         <is>
-          <t>10:00:00</t>
+          <t>14:00:00</t>
         </is>
       </c>
       <c r="G62" s="5" t="n">
@@ -2660,12 +2660,12 @@
       </c>
       <c r="B63" s="6" t="inlineStr">
         <is>
-          <t>B2</t>
+          <t>B1</t>
         </is>
       </c>
       <c r="C63" s="6" t="inlineStr">
         <is>
-          <t>parasitology sgd/pos</t>
+          <t>histology</t>
         </is>
       </c>
       <c r="D63" s="6" t="inlineStr">
@@ -2675,7 +2675,7 @@
       </c>
       <c r="E63" s="7" t="inlineStr">
         <is>
-          <t>10/12/2025</t>
+          <t>10/11/2025</t>
         </is>
       </c>
       <c r="F63" s="8" t="inlineStr">
@@ -2695,27 +2695,27 @@
       </c>
       <c r="B64" s="2" t="inlineStr">
         <is>
-          <t>B2</t>
+          <t>B1</t>
         </is>
       </c>
       <c r="C64" s="2" t="inlineStr">
         <is>
-          <t>pathology lab/museum</t>
+          <t>histology</t>
         </is>
       </c>
       <c r="D64" s="2" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>2</t>
         </is>
       </c>
       <c r="E64" s="3" t="inlineStr">
         <is>
-          <t>04/12/2025</t>
+          <t>03/12/2025</t>
         </is>
       </c>
       <c r="F64" s="4" t="inlineStr">
         <is>
-          <t>10:00:00</t>
+          <t>14:00:00</t>
         </is>
       </c>
       <c r="G64" s="5" t="n">
@@ -2730,27 +2730,27 @@
       </c>
       <c r="B65" s="6" t="inlineStr">
         <is>
-          <t>B2</t>
+          <t>B1</t>
         </is>
       </c>
       <c r="C65" s="6" t="inlineStr">
         <is>
-          <t>pharmacology</t>
+          <t>histology</t>
         </is>
       </c>
       <c r="D65" s="6" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>3</t>
         </is>
       </c>
       <c r="E65" s="7" t="inlineStr">
         <is>
-          <t>04/12/2025</t>
+          <t>11/12/2025</t>
         </is>
       </c>
       <c r="F65" s="8" t="inlineStr">
         <is>
-          <t>14:00:00</t>
+          <t>10:00:00</t>
         </is>
       </c>
       <c r="G65" s="9" t="n">
@@ -2765,27 +2765,27 @@
       </c>
       <c r="B66" s="2" t="inlineStr">
         <is>
-          <t>B2</t>
+          <t>B1</t>
         </is>
       </c>
       <c r="C66" s="2" t="inlineStr">
         <is>
-          <t>pharmacology</t>
+          <t>microbiology</t>
         </is>
       </c>
       <c r="D66" s="2" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>1</t>
         </is>
       </c>
       <c r="E66" s="3" t="inlineStr">
         <is>
-          <t>08/12/2025</t>
+          <t>24/11/2025</t>
         </is>
       </c>
       <c r="F66" s="4" t="inlineStr">
         <is>
-          <t>12:00:00</t>
+          <t>14:00:00</t>
         </is>
       </c>
       <c r="G66" s="5" t="n">
@@ -2800,31 +2800,31 @@
       </c>
       <c r="B67" s="6" t="inlineStr">
         <is>
-          <t>B2</t>
+          <t>B1</t>
         </is>
       </c>
       <c r="C67" s="6" t="inlineStr">
         <is>
-          <t>physiology</t>
+          <t>microbiology</t>
         </is>
       </c>
       <c r="D67" s="6" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>2</t>
         </is>
       </c>
       <c r="E67" s="7" t="inlineStr">
         <is>
-          <t>12/11/2025</t>
+          <t>10/12/2025</t>
         </is>
       </c>
       <c r="F67" s="8" t="inlineStr">
         <is>
-          <t>12:00:00</t>
+          <t>14:00:00</t>
         </is>
       </c>
       <c r="G67" s="9" t="n">
-        <v>90</v>
+        <v>120</v>
       </c>
     </row>
     <row r="68">
@@ -2835,31 +2835,31 @@
       </c>
       <c r="B68" s="2" t="inlineStr">
         <is>
-          <t>B2</t>
+          <t>B1</t>
         </is>
       </c>
       <c r="C68" s="2" t="inlineStr">
         <is>
-          <t>physiology</t>
+          <t>parasitology sgd/pos</t>
         </is>
       </c>
       <c r="D68" s="2" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>1</t>
         </is>
       </c>
       <c r="E68" s="3" t="inlineStr">
         <is>
-          <t>19/11/2025</t>
+          <t>10/12/2025</t>
         </is>
       </c>
       <c r="F68" s="4" t="inlineStr">
         <is>
-          <t>13:00:00</t>
+          <t>12:00:00</t>
         </is>
       </c>
       <c r="G68" s="5" t="n">
-        <v>90</v>
+        <v>120</v>
       </c>
     </row>
     <row r="69">
@@ -2870,31 +2870,31 @@
       </c>
       <c r="B69" s="6" t="inlineStr">
         <is>
-          <t>B2</t>
+          <t>B1</t>
         </is>
       </c>
       <c r="C69" s="6" t="inlineStr">
         <is>
-          <t>physiology</t>
+          <t>pathology lab/museum</t>
         </is>
       </c>
       <c r="D69" s="6" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>1</t>
         </is>
       </c>
       <c r="E69" s="7" t="inlineStr">
         <is>
-          <t>20/11/2025</t>
+          <t>03/12/2025</t>
         </is>
       </c>
       <c r="F69" s="8" t="inlineStr">
         <is>
-          <t>10:00:00</t>
+          <t>14:00:00</t>
         </is>
       </c>
       <c r="G69" s="9" t="n">
-        <v>90</v>
+        <v>120</v>
       </c>
     </row>
     <row r="70">
@@ -2905,31 +2905,31 @@
       </c>
       <c r="B70" s="2" t="inlineStr">
         <is>
-          <t>B3</t>
+          <t>B1</t>
         </is>
       </c>
       <c r="C70" s="2" t="inlineStr">
         <is>
-          <t>anatomy</t>
+          <t>pathology lab/museum</t>
         </is>
       </c>
       <c r="D70" s="2" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>2</t>
         </is>
       </c>
       <c r="E70" s="3" t="inlineStr">
         <is>
-          <t>13/11/2025</t>
+          <t>11/12/2025</t>
         </is>
       </c>
       <c r="F70" s="4" t="inlineStr">
         <is>
-          <t>13:00:00</t>
+          <t>08:00:00</t>
         </is>
       </c>
       <c r="G70" s="5" t="n">
-        <v>90</v>
+        <v>120</v>
       </c>
     </row>
     <row r="71">
@@ -2940,22 +2940,22 @@
       </c>
       <c r="B71" s="6" t="inlineStr">
         <is>
-          <t>B3</t>
+          <t>B1</t>
         </is>
       </c>
       <c r="C71" s="6" t="inlineStr">
         <is>
-          <t>biochemistry lab/cbl</t>
+          <t>pathology lab/museum</t>
         </is>
       </c>
       <c r="D71" s="6" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>3</t>
         </is>
       </c>
       <c r="E71" s="7" t="inlineStr">
         <is>
-          <t>19/11/2025</t>
+          <t>15/12/2025</t>
         </is>
       </c>
       <c r="F71" s="8" t="inlineStr">
@@ -2975,27 +2975,27 @@
       </c>
       <c r="B72" s="2" t="inlineStr">
         <is>
-          <t>B3</t>
+          <t>B1</t>
         </is>
       </c>
       <c r="C72" s="2" t="inlineStr">
         <is>
-          <t>histology</t>
+          <t>pathology lab/museum</t>
         </is>
       </c>
       <c r="D72" s="2" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>4</t>
         </is>
       </c>
       <c r="E72" s="3" t="inlineStr">
         <is>
-          <t>10/11/2025</t>
+          <t>15/12/2025</t>
         </is>
       </c>
       <c r="F72" s="4" t="inlineStr">
         <is>
-          <t>12:00:00</t>
+          <t>14:00:00</t>
         </is>
       </c>
       <c r="G72" s="5" t="n">
@@ -3010,27 +3010,27 @@
       </c>
       <c r="B73" s="6" t="inlineStr">
         <is>
-          <t>B3</t>
+          <t>B1</t>
         </is>
       </c>
       <c r="C73" s="6" t="inlineStr">
         <is>
-          <t>histology</t>
+          <t>pharmacology</t>
         </is>
       </c>
       <c r="D73" s="6" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>1</t>
         </is>
       </c>
       <c r="E73" s="7" t="inlineStr">
         <is>
-          <t>04/12/2025</t>
+          <t>01/12/2025</t>
         </is>
       </c>
       <c r="F73" s="8" t="inlineStr">
         <is>
-          <t>08:00:00</t>
+          <t>14:00:00</t>
         </is>
       </c>
       <c r="G73" s="9" t="n">
@@ -3045,27 +3045,27 @@
       </c>
       <c r="B74" s="2" t="inlineStr">
         <is>
-          <t>B3</t>
+          <t>B1</t>
         </is>
       </c>
       <c r="C74" s="2" t="inlineStr">
         <is>
-          <t>histology</t>
+          <t>pharmacology</t>
         </is>
       </c>
       <c r="D74" s="2" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>2</t>
         </is>
       </c>
       <c r="E74" s="3" t="inlineStr">
         <is>
-          <t>11/12/2025</t>
+          <t>08/12/2025</t>
         </is>
       </c>
       <c r="F74" s="4" t="inlineStr">
         <is>
-          <t>12:00:00</t>
+          <t>14:00:00</t>
         </is>
       </c>
       <c r="G74" s="5" t="n">
@@ -3080,12 +3080,12 @@
       </c>
       <c r="B75" s="6" t="inlineStr">
         <is>
-          <t>B3</t>
+          <t>B1</t>
         </is>
       </c>
       <c r="C75" s="6" t="inlineStr">
         <is>
-          <t>microbiology</t>
+          <t>physiology</t>
         </is>
       </c>
       <c r="D75" s="6" t="inlineStr">
@@ -3095,16 +3095,16 @@
       </c>
       <c r="E75" s="7" t="inlineStr">
         <is>
-          <t>25/11/2025</t>
+          <t>12/11/2025</t>
         </is>
       </c>
       <c r="F75" s="8" t="inlineStr">
         <is>
-          <t>10:00:00</t>
+          <t>13:00:00</t>
         </is>
       </c>
       <c r="G75" s="9" t="n">
-        <v>120</v>
+        <v>90</v>
       </c>
     </row>
     <row r="76">
@@ -3115,12 +3115,12 @@
       </c>
       <c r="B76" s="2" t="inlineStr">
         <is>
-          <t>B3</t>
+          <t>B1</t>
         </is>
       </c>
       <c r="C76" s="2" t="inlineStr">
         <is>
-          <t>microbiology</t>
+          <t>physiology</t>
         </is>
       </c>
       <c r="D76" s="2" t="inlineStr">
@@ -3130,7 +3130,7 @@
       </c>
       <c r="E76" s="3" t="inlineStr">
         <is>
-          <t>08/12/2025</t>
+          <t>19/11/2025</t>
         </is>
       </c>
       <c r="F76" s="4" t="inlineStr">
@@ -3139,7 +3139,7 @@
         </is>
       </c>
       <c r="G76" s="5" t="n">
-        <v>120</v>
+        <v>90</v>
       </c>
     </row>
     <row r="77">
@@ -3150,31 +3150,31 @@
       </c>
       <c r="B77" s="6" t="inlineStr">
         <is>
-          <t>B3</t>
+          <t>B1</t>
         </is>
       </c>
       <c r="C77" s="6" t="inlineStr">
         <is>
-          <t>parasitology sgd/pos</t>
+          <t>physiology</t>
         </is>
       </c>
       <c r="D77" s="6" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>3</t>
         </is>
       </c>
       <c r="E77" s="7" t="inlineStr">
         <is>
-          <t>08/12/2025</t>
+          <t>20/11/2025</t>
         </is>
       </c>
       <c r="F77" s="8" t="inlineStr">
         <is>
-          <t>14:00:00</t>
+          <t>11:00:00</t>
         </is>
       </c>
       <c r="G77" s="9" t="n">
-        <v>120</v>
+        <v>90</v>
       </c>
     </row>
     <row r="78">
@@ -3185,12 +3185,12 @@
       </c>
       <c r="B78" s="2" t="inlineStr">
         <is>
-          <t>B3</t>
+          <t>B2</t>
         </is>
       </c>
       <c r="C78" s="2" t="inlineStr">
         <is>
-          <t>pathology lab/museum</t>
+          <t>anatomy</t>
         </is>
       </c>
       <c r="D78" s="2" t="inlineStr">
@@ -3200,16 +3200,16 @@
       </c>
       <c r="E78" s="3" t="inlineStr">
         <is>
-          <t>03/12/2025</t>
+          <t>13/11/2025</t>
         </is>
       </c>
       <c r="F78" s="4" t="inlineStr">
         <is>
-          <t>12:00:00</t>
+          <t>14:00:00</t>
         </is>
       </c>
       <c r="G78" s="5" t="n">
-        <v>120</v>
+        <v>90</v>
       </c>
     </row>
     <row r="79">
@@ -3220,22 +3220,22 @@
       </c>
       <c r="B79" s="6" t="inlineStr">
         <is>
-          <t>B3</t>
+          <t>B2</t>
         </is>
       </c>
       <c r="C79" s="6" t="inlineStr">
         <is>
-          <t>pharmacology</t>
+          <t>anatomy</t>
         </is>
       </c>
       <c r="D79" s="6" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>2</t>
         </is>
       </c>
       <c r="E79" s="7" t="inlineStr">
         <is>
-          <t>04/12/2025</t>
+          <t>11/12/2025</t>
         </is>
       </c>
       <c r="F79" s="8" t="inlineStr">
@@ -3255,27 +3255,27 @@
       </c>
       <c r="B80" s="2" t="inlineStr">
         <is>
-          <t>B3</t>
+          <t>B2</t>
         </is>
       </c>
       <c r="C80" s="2" t="inlineStr">
         <is>
-          <t>pharmacology</t>
+          <t>anatomy</t>
         </is>
       </c>
       <c r="D80" s="2" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>3</t>
         </is>
       </c>
       <c r="E80" s="3" t="inlineStr">
         <is>
-          <t>10/12/2025</t>
+          <t>17/12/2025</t>
         </is>
       </c>
       <c r="F80" s="4" t="inlineStr">
         <is>
-          <t>14:00:00</t>
+          <t>10:00:00</t>
         </is>
       </c>
       <c r="G80" s="5" t="n">
@@ -3290,12 +3290,12 @@
       </c>
       <c r="B81" s="6" t="inlineStr">
         <is>
-          <t>B3</t>
+          <t>B2</t>
         </is>
       </c>
       <c r="C81" s="6" t="inlineStr">
         <is>
-          <t>physiology</t>
+          <t>biochemistry lab/cbl</t>
         </is>
       </c>
       <c r="D81" s="6" t="inlineStr">
@@ -3305,7 +3305,7 @@
       </c>
       <c r="E81" s="7" t="inlineStr">
         <is>
-          <t>12/11/2025</t>
+          <t>24/11/2025</t>
         </is>
       </c>
       <c r="F81" s="8" t="inlineStr">
@@ -3314,7 +3314,7 @@
         </is>
       </c>
       <c r="G81" s="9" t="n">
-        <v>90</v>
+        <v>120</v>
       </c>
     </row>
     <row r="82">
@@ -3325,31 +3325,31 @@
       </c>
       <c r="B82" s="2" t="inlineStr">
         <is>
-          <t>B3</t>
+          <t>B2</t>
         </is>
       </c>
       <c r="C82" s="2" t="inlineStr">
         <is>
-          <t>physiology</t>
+          <t>histology</t>
         </is>
       </c>
       <c r="D82" s="2" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>1</t>
         </is>
       </c>
       <c r="E82" s="3" t="inlineStr">
         <is>
-          <t>19/11/2025</t>
+          <t>13/11/2025</t>
         </is>
       </c>
       <c r="F82" s="4" t="inlineStr">
         <is>
-          <t>14:00:00</t>
+          <t>12:00:00</t>
         </is>
       </c>
       <c r="G82" s="5" t="n">
-        <v>90</v>
+        <v>120</v>
       </c>
     </row>
     <row r="83">
@@ -3360,30 +3360,1150 @@
       </c>
       <c r="B83" s="6" t="inlineStr">
         <is>
+          <t>B2</t>
+        </is>
+      </c>
+      <c r="C83" s="6" t="inlineStr">
+        <is>
+          <t>histology</t>
+        </is>
+      </c>
+      <c r="D83" s="6" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="E83" s="7" t="inlineStr">
+        <is>
+          <t>01/12/2025</t>
+        </is>
+      </c>
+      <c r="F83" s="8" t="inlineStr">
+        <is>
+          <t>14:00:00</t>
+        </is>
+      </c>
+      <c r="G83" s="9" t="n">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="84">
+      <c r="A84" s="2" t="inlineStr">
+        <is>
+          <t>Year 3</t>
+        </is>
+      </c>
+      <c r="B84" s="2" t="inlineStr">
+        <is>
+          <t>B2</t>
+        </is>
+      </c>
+      <c r="C84" s="2" t="inlineStr">
+        <is>
+          <t>histology</t>
+        </is>
+      </c>
+      <c r="D84" s="2" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
+      <c r="E84" s="3" t="inlineStr">
+        <is>
+          <t>11/12/2025</t>
+        </is>
+      </c>
+      <c r="F84" s="4" t="inlineStr">
+        <is>
+          <t>14:00:00</t>
+        </is>
+      </c>
+      <c r="G84" s="5" t="n">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="85">
+      <c r="A85" s="6" t="inlineStr">
+        <is>
+          <t>Year 3</t>
+        </is>
+      </c>
+      <c r="B85" s="6" t="inlineStr">
+        <is>
+          <t>B2</t>
+        </is>
+      </c>
+      <c r="C85" s="6" t="inlineStr">
+        <is>
+          <t>microbiology</t>
+        </is>
+      </c>
+      <c r="D85" s="6" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="E85" s="7" t="inlineStr">
+        <is>
+          <t>24/11/2025</t>
+        </is>
+      </c>
+      <c r="F85" s="8" t="inlineStr">
+        <is>
+          <t>12:00:00</t>
+        </is>
+      </c>
+      <c r="G85" s="9" t="n">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="86">
+      <c r="A86" s="2" t="inlineStr">
+        <is>
+          <t>Year 3</t>
+        </is>
+      </c>
+      <c r="B86" s="2" t="inlineStr">
+        <is>
+          <t>B2</t>
+        </is>
+      </c>
+      <c r="C86" s="2" t="inlineStr">
+        <is>
+          <t>microbiology</t>
+        </is>
+      </c>
+      <c r="D86" s="2" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="E86" s="3" t="inlineStr">
+        <is>
+          <t>09/12/2025</t>
+        </is>
+      </c>
+      <c r="F86" s="4" t="inlineStr">
+        <is>
+          <t>10:00:00</t>
+        </is>
+      </c>
+      <c r="G86" s="5" t="n">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="87">
+      <c r="A87" s="6" t="inlineStr">
+        <is>
+          <t>Year 3</t>
+        </is>
+      </c>
+      <c r="B87" s="6" t="inlineStr">
+        <is>
+          <t>B2</t>
+        </is>
+      </c>
+      <c r="C87" s="6" t="inlineStr">
+        <is>
+          <t>parasitology sgd/pos</t>
+        </is>
+      </c>
+      <c r="D87" s="6" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="E87" s="7" t="inlineStr">
+        <is>
+          <t>10/12/2025</t>
+        </is>
+      </c>
+      <c r="F87" s="8" t="inlineStr">
+        <is>
+          <t>14:00:00</t>
+        </is>
+      </c>
+      <c r="G87" s="9" t="n">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="88">
+      <c r="A88" s="2" t="inlineStr">
+        <is>
+          <t>Year 3</t>
+        </is>
+      </c>
+      <c r="B88" s="2" t="inlineStr">
+        <is>
+          <t>B2</t>
+        </is>
+      </c>
+      <c r="C88" s="2" t="inlineStr">
+        <is>
+          <t>pathology lab/museum</t>
+        </is>
+      </c>
+      <c r="D88" s="2" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="E88" s="3" t="inlineStr">
+        <is>
+          <t>04/12/2025</t>
+        </is>
+      </c>
+      <c r="F88" s="4" t="inlineStr">
+        <is>
+          <t>10:00:00</t>
+        </is>
+      </c>
+      <c r="G88" s="5" t="n">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="89">
+      <c r="A89" s="6" t="inlineStr">
+        <is>
+          <t>Year 3</t>
+        </is>
+      </c>
+      <c r="B89" s="6" t="inlineStr">
+        <is>
+          <t>B2</t>
+        </is>
+      </c>
+      <c r="C89" s="6" t="inlineStr">
+        <is>
+          <t>pathology lab/museum</t>
+        </is>
+      </c>
+      <c r="D89" s="6" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="E89" s="7" t="inlineStr">
+        <is>
+          <t>07/12/2025</t>
+        </is>
+      </c>
+      <c r="F89" s="8" t="inlineStr">
+        <is>
+          <t>10:00:00</t>
+        </is>
+      </c>
+      <c r="G89" s="9" t="n">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="90">
+      <c r="A90" s="2" t="inlineStr">
+        <is>
+          <t>Year 3</t>
+        </is>
+      </c>
+      <c r="B90" s="2" t="inlineStr">
+        <is>
+          <t>B2</t>
+        </is>
+      </c>
+      <c r="C90" s="2" t="inlineStr">
+        <is>
+          <t>pathology lab/museum</t>
+        </is>
+      </c>
+      <c r="D90" s="2" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
+      <c r="E90" s="3" t="inlineStr">
+        <is>
+          <t>15/12/2025</t>
+        </is>
+      </c>
+      <c r="F90" s="4" t="inlineStr">
+        <is>
+          <t>14:00:00</t>
+        </is>
+      </c>
+      <c r="G90" s="5" t="n">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="91">
+      <c r="A91" s="6" t="inlineStr">
+        <is>
+          <t>Year 3</t>
+        </is>
+      </c>
+      <c r="B91" s="6" t="inlineStr">
+        <is>
+          <t>B2</t>
+        </is>
+      </c>
+      <c r="C91" s="6" t="inlineStr">
+        <is>
+          <t>pathology lab/museum</t>
+        </is>
+      </c>
+      <c r="D91" s="6" t="inlineStr">
+        <is>
+          <t>4</t>
+        </is>
+      </c>
+      <c r="E91" s="7" t="inlineStr">
+        <is>
+          <t>15/12/2025</t>
+        </is>
+      </c>
+      <c r="F91" s="8" t="inlineStr">
+        <is>
+          <t>12:00:00</t>
+        </is>
+      </c>
+      <c r="G91" s="9" t="n">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="92">
+      <c r="A92" s="2" t="inlineStr">
+        <is>
+          <t>Year 3</t>
+        </is>
+      </c>
+      <c r="B92" s="2" t="inlineStr">
+        <is>
+          <t>B2</t>
+        </is>
+      </c>
+      <c r="C92" s="2" t="inlineStr">
+        <is>
+          <t>pharmacology</t>
+        </is>
+      </c>
+      <c r="D92" s="2" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="E92" s="3" t="inlineStr">
+        <is>
+          <t>04/12/2025</t>
+        </is>
+      </c>
+      <c r="F92" s="4" t="inlineStr">
+        <is>
+          <t>14:00:00</t>
+        </is>
+      </c>
+      <c r="G92" s="5" t="n">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="93">
+      <c r="A93" s="6" t="inlineStr">
+        <is>
+          <t>Year 3</t>
+        </is>
+      </c>
+      <c r="B93" s="6" t="inlineStr">
+        <is>
+          <t>B2</t>
+        </is>
+      </c>
+      <c r="C93" s="6" t="inlineStr">
+        <is>
+          <t>pharmacology</t>
+        </is>
+      </c>
+      <c r="D93" s="6" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="E93" s="7" t="inlineStr">
+        <is>
+          <t>08/12/2025</t>
+        </is>
+      </c>
+      <c r="F93" s="8" t="inlineStr">
+        <is>
+          <t>12:00:00</t>
+        </is>
+      </c>
+      <c r="G93" s="9" t="n">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="94">
+      <c r="A94" s="2" t="inlineStr">
+        <is>
+          <t>Year 3</t>
+        </is>
+      </c>
+      <c r="B94" s="2" t="inlineStr">
+        <is>
+          <t>B2</t>
+        </is>
+      </c>
+      <c r="C94" s="2" t="inlineStr">
+        <is>
+          <t>physiology</t>
+        </is>
+      </c>
+      <c r="D94" s="2" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="E94" s="3" t="inlineStr">
+        <is>
+          <t>12/11/2025</t>
+        </is>
+      </c>
+      <c r="F94" s="4" t="inlineStr">
+        <is>
+          <t>12:00:00</t>
+        </is>
+      </c>
+      <c r="G94" s="5" t="n">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="95">
+      <c r="A95" s="6" t="inlineStr">
+        <is>
+          <t>Year 3</t>
+        </is>
+      </c>
+      <c r="B95" s="6" t="inlineStr">
+        <is>
+          <t>B2</t>
+        </is>
+      </c>
+      <c r="C95" s="6" t="inlineStr">
+        <is>
+          <t>physiology</t>
+        </is>
+      </c>
+      <c r="D95" s="6" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="E95" s="7" t="inlineStr">
+        <is>
+          <t>19/11/2025</t>
+        </is>
+      </c>
+      <c r="F95" s="8" t="inlineStr">
+        <is>
+          <t>13:00:00</t>
+        </is>
+      </c>
+      <c r="G95" s="9" t="n">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="96">
+      <c r="A96" s="2" t="inlineStr">
+        <is>
+          <t>Year 3</t>
+        </is>
+      </c>
+      <c r="B96" s="2" t="inlineStr">
+        <is>
+          <t>B2</t>
+        </is>
+      </c>
+      <c r="C96" s="2" t="inlineStr">
+        <is>
+          <t>physiology</t>
+        </is>
+      </c>
+      <c r="D96" s="2" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
+      <c r="E96" s="3" t="inlineStr">
+        <is>
+          <t>20/11/2025</t>
+        </is>
+      </c>
+      <c r="F96" s="4" t="inlineStr">
+        <is>
+          <t>10:00:00</t>
+        </is>
+      </c>
+      <c r="G96" s="5" t="n">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="97">
+      <c r="A97" s="6" t="inlineStr">
+        <is>
+          <t>Year 3</t>
+        </is>
+      </c>
+      <c r="B97" s="6" t="inlineStr">
+        <is>
           <t>B3</t>
         </is>
       </c>
-      <c r="C83" s="6" t="inlineStr">
+      <c r="C97" s="6" t="inlineStr">
+        <is>
+          <t>anatomy</t>
+        </is>
+      </c>
+      <c r="D97" s="6" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="E97" s="7" t="inlineStr">
+        <is>
+          <t>13/11/2025</t>
+        </is>
+      </c>
+      <c r="F97" s="8" t="inlineStr">
+        <is>
+          <t>13:00:00</t>
+        </is>
+      </c>
+      <c r="G97" s="9" t="n">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="98">
+      <c r="A98" s="2" t="inlineStr">
+        <is>
+          <t>Year 3</t>
+        </is>
+      </c>
+      <c r="B98" s="2" t="inlineStr">
+        <is>
+          <t>B3</t>
+        </is>
+      </c>
+      <c r="C98" s="2" t="inlineStr">
+        <is>
+          <t>anatomy</t>
+        </is>
+      </c>
+      <c r="D98" s="2" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="E98" s="3" t="inlineStr">
+        <is>
+          <t>11/12/2025</t>
+        </is>
+      </c>
+      <c r="F98" s="4" t="inlineStr">
+        <is>
+          <t>08:00:00</t>
+        </is>
+      </c>
+      <c r="G98" s="5" t="n">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="99">
+      <c r="A99" s="6" t="inlineStr">
+        <is>
+          <t>Year 3</t>
+        </is>
+      </c>
+      <c r="B99" s="6" t="inlineStr">
+        <is>
+          <t>B3</t>
+        </is>
+      </c>
+      <c r="C99" s="6" t="inlineStr">
+        <is>
+          <t>anatomy</t>
+        </is>
+      </c>
+      <c r="D99" s="6" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
+      <c r="E99" s="7" t="inlineStr">
+        <is>
+          <t>16/12/2025</t>
+        </is>
+      </c>
+      <c r="F99" s="8" t="inlineStr">
+        <is>
+          <t>08:00:00</t>
+        </is>
+      </c>
+      <c r="G99" s="9" t="n">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="100">
+      <c r="A100" s="2" t="inlineStr">
+        <is>
+          <t>Year 3</t>
+        </is>
+      </c>
+      <c r="B100" s="2" t="inlineStr">
+        <is>
+          <t>B3</t>
+        </is>
+      </c>
+      <c r="C100" s="2" t="inlineStr">
+        <is>
+          <t>biochemistry lab/cbl</t>
+        </is>
+      </c>
+      <c r="D100" s="2" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="E100" s="3" t="inlineStr">
+        <is>
+          <t>19/11/2025</t>
+        </is>
+      </c>
+      <c r="F100" s="4" t="inlineStr">
+        <is>
+          <t>12:00:00</t>
+        </is>
+      </c>
+      <c r="G100" s="5" t="n">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="101">
+      <c r="A101" s="6" t="inlineStr">
+        <is>
+          <t>Year 3</t>
+        </is>
+      </c>
+      <c r="B101" s="6" t="inlineStr">
+        <is>
+          <t>B3</t>
+        </is>
+      </c>
+      <c r="C101" s="6" t="inlineStr">
+        <is>
+          <t>histology</t>
+        </is>
+      </c>
+      <c r="D101" s="6" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="E101" s="7" t="inlineStr">
+        <is>
+          <t>10/11/2025</t>
+        </is>
+      </c>
+      <c r="F101" s="8" t="inlineStr">
+        <is>
+          <t>12:00:00</t>
+        </is>
+      </c>
+      <c r="G101" s="9" t="n">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="102">
+      <c r="A102" s="2" t="inlineStr">
+        <is>
+          <t>Year 3</t>
+        </is>
+      </c>
+      <c r="B102" s="2" t="inlineStr">
+        <is>
+          <t>B3</t>
+        </is>
+      </c>
+      <c r="C102" s="2" t="inlineStr">
+        <is>
+          <t>histology</t>
+        </is>
+      </c>
+      <c r="D102" s="2" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="E102" s="3" t="inlineStr">
+        <is>
+          <t>04/12/2025</t>
+        </is>
+      </c>
+      <c r="F102" s="4" t="inlineStr">
+        <is>
+          <t>08:00:00</t>
+        </is>
+      </c>
+      <c r="G102" s="5" t="n">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="103">
+      <c r="A103" s="6" t="inlineStr">
+        <is>
+          <t>Year 3</t>
+        </is>
+      </c>
+      <c r="B103" s="6" t="inlineStr">
+        <is>
+          <t>B3</t>
+        </is>
+      </c>
+      <c r="C103" s="6" t="inlineStr">
+        <is>
+          <t>histology</t>
+        </is>
+      </c>
+      <c r="D103" s="6" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
+      <c r="E103" s="7" t="inlineStr">
+        <is>
+          <t>11/12/2025</t>
+        </is>
+      </c>
+      <c r="F103" s="8" t="inlineStr">
+        <is>
+          <t>12:00:00</t>
+        </is>
+      </c>
+      <c r="G103" s="9" t="n">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="104">
+      <c r="A104" s="2" t="inlineStr">
+        <is>
+          <t>Year 3</t>
+        </is>
+      </c>
+      <c r="B104" s="2" t="inlineStr">
+        <is>
+          <t>B3</t>
+        </is>
+      </c>
+      <c r="C104" s="2" t="inlineStr">
+        <is>
+          <t>microbiology</t>
+        </is>
+      </c>
+      <c r="D104" s="2" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="E104" s="3" t="inlineStr">
+        <is>
+          <t>25/11/2025</t>
+        </is>
+      </c>
+      <c r="F104" s="4" t="inlineStr">
+        <is>
+          <t>10:00:00</t>
+        </is>
+      </c>
+      <c r="G104" s="5" t="n">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="105">
+      <c r="A105" s="6" t="inlineStr">
+        <is>
+          <t>Year 3</t>
+        </is>
+      </c>
+      <c r="B105" s="6" t="inlineStr">
+        <is>
+          <t>B3</t>
+        </is>
+      </c>
+      <c r="C105" s="6" t="inlineStr">
+        <is>
+          <t>microbiology</t>
+        </is>
+      </c>
+      <c r="D105" s="6" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="E105" s="7" t="inlineStr">
+        <is>
+          <t>08/12/2025</t>
+        </is>
+      </c>
+      <c r="F105" s="8" t="inlineStr">
+        <is>
+          <t>12:00:00</t>
+        </is>
+      </c>
+      <c r="G105" s="9" t="n">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="106">
+      <c r="A106" s="2" t="inlineStr">
+        <is>
+          <t>Year 3</t>
+        </is>
+      </c>
+      <c r="B106" s="2" t="inlineStr">
+        <is>
+          <t>B3</t>
+        </is>
+      </c>
+      <c r="C106" s="2" t="inlineStr">
+        <is>
+          <t>parasitology sgd/pos</t>
+        </is>
+      </c>
+      <c r="D106" s="2" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="E106" s="3" t="inlineStr">
+        <is>
+          <t>08/12/2025</t>
+        </is>
+      </c>
+      <c r="F106" s="4" t="inlineStr">
+        <is>
+          <t>14:00:00</t>
+        </is>
+      </c>
+      <c r="G106" s="5" t="n">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="107">
+      <c r="A107" s="6" t="inlineStr">
+        <is>
+          <t>Year 3</t>
+        </is>
+      </c>
+      <c r="B107" s="6" t="inlineStr">
+        <is>
+          <t>B3</t>
+        </is>
+      </c>
+      <c r="C107" s="6" t="inlineStr">
+        <is>
+          <t>pathology lab/museum</t>
+        </is>
+      </c>
+      <c r="D107" s="6" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="E107" s="7" t="inlineStr">
+        <is>
+          <t>03/12/2025</t>
+        </is>
+      </c>
+      <c r="F107" s="8" t="inlineStr">
+        <is>
+          <t>12:00:00</t>
+        </is>
+      </c>
+      <c r="G107" s="9" t="n">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="108">
+      <c r="A108" s="2" t="inlineStr">
+        <is>
+          <t>Year 3</t>
+        </is>
+      </c>
+      <c r="B108" s="2" t="inlineStr">
+        <is>
+          <t>B3</t>
+        </is>
+      </c>
+      <c r="C108" s="2" t="inlineStr">
+        <is>
+          <t>pathology lab/museum</t>
+        </is>
+      </c>
+      <c r="D108" s="2" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="E108" s="3" t="inlineStr">
+        <is>
+          <t>10/12/2025</t>
+        </is>
+      </c>
+      <c r="F108" s="4" t="inlineStr">
+        <is>
+          <t>12:00:00</t>
+        </is>
+      </c>
+      <c r="G108" s="5" t="n">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="109">
+      <c r="A109" s="6" t="inlineStr">
+        <is>
+          <t>Year 3</t>
+        </is>
+      </c>
+      <c r="B109" s="6" t="inlineStr">
+        <is>
+          <t>B3</t>
+        </is>
+      </c>
+      <c r="C109" s="6" t="inlineStr">
+        <is>
+          <t>pathology lab/museum</t>
+        </is>
+      </c>
+      <c r="D109" s="6" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
+      <c r="E109" s="7" t="inlineStr">
+        <is>
+          <t>17/12/2025</t>
+        </is>
+      </c>
+      <c r="F109" s="8" t="inlineStr">
+        <is>
+          <t>12:00:00</t>
+        </is>
+      </c>
+      <c r="G109" s="9" t="n">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="110">
+      <c r="A110" s="2" t="inlineStr">
+        <is>
+          <t>Year 3</t>
+        </is>
+      </c>
+      <c r="B110" s="2" t="inlineStr">
+        <is>
+          <t>B3</t>
+        </is>
+      </c>
+      <c r="C110" s="2" t="inlineStr">
+        <is>
+          <t>pathology lab/museum</t>
+        </is>
+      </c>
+      <c r="D110" s="2" t="inlineStr">
+        <is>
+          <t>4</t>
+        </is>
+      </c>
+      <c r="E110" s="3" t="inlineStr">
+        <is>
+          <t>17/12/2025</t>
+        </is>
+      </c>
+      <c r="F110" s="4" t="inlineStr">
+        <is>
+          <t>14:00:00</t>
+        </is>
+      </c>
+      <c r="G110" s="5" t="n">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="111">
+      <c r="A111" s="6" t="inlineStr">
+        <is>
+          <t>Year 3</t>
+        </is>
+      </c>
+      <c r="B111" s="6" t="inlineStr">
+        <is>
+          <t>B3</t>
+        </is>
+      </c>
+      <c r="C111" s="6" t="inlineStr">
+        <is>
+          <t>pharmacology</t>
+        </is>
+      </c>
+      <c r="D111" s="6" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="E111" s="7" t="inlineStr">
+        <is>
+          <t>04/12/2025</t>
+        </is>
+      </c>
+      <c r="F111" s="8" t="inlineStr">
+        <is>
+          <t>12:00:00</t>
+        </is>
+      </c>
+      <c r="G111" s="9" t="n">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="112">
+      <c r="A112" s="2" t="inlineStr">
+        <is>
+          <t>Year 3</t>
+        </is>
+      </c>
+      <c r="B112" s="2" t="inlineStr">
+        <is>
+          <t>B3</t>
+        </is>
+      </c>
+      <c r="C112" s="2" t="inlineStr">
+        <is>
+          <t>pharmacology</t>
+        </is>
+      </c>
+      <c r="D112" s="2" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="E112" s="3" t="inlineStr">
+        <is>
+          <t>10/12/2025</t>
+        </is>
+      </c>
+      <c r="F112" s="4" t="inlineStr">
+        <is>
+          <t>14:00:00</t>
+        </is>
+      </c>
+      <c r="G112" s="5" t="n">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="113">
+      <c r="A113" s="6" t="inlineStr">
+        <is>
+          <t>Year 3</t>
+        </is>
+      </c>
+      <c r="B113" s="6" t="inlineStr">
+        <is>
+          <t>B3</t>
+        </is>
+      </c>
+      <c r="C113" s="6" t="inlineStr">
         <is>
           <t>physiology</t>
         </is>
       </c>
-      <c r="D83" s="6" t="inlineStr">
+      <c r="D113" s="6" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="E113" s="7" t="inlineStr">
+        <is>
+          <t>12/11/2025</t>
+        </is>
+      </c>
+      <c r="F113" s="8" t="inlineStr">
+        <is>
+          <t>14:00:00</t>
+        </is>
+      </c>
+      <c r="G113" s="9" t="n">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="114">
+      <c r="A114" s="2" t="inlineStr">
+        <is>
+          <t>Year 3</t>
+        </is>
+      </c>
+      <c r="B114" s="2" t="inlineStr">
+        <is>
+          <t>B3</t>
+        </is>
+      </c>
+      <c r="C114" s="2" t="inlineStr">
+        <is>
+          <t>physiology</t>
+        </is>
+      </c>
+      <c r="D114" s="2" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="E114" s="3" t="inlineStr">
+        <is>
+          <t>19/11/2025</t>
+        </is>
+      </c>
+      <c r="F114" s="4" t="inlineStr">
+        <is>
+          <t>14:00:00</t>
+        </is>
+      </c>
+      <c r="G114" s="5" t="n">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="115">
+      <c r="A115" s="6" t="inlineStr">
+        <is>
+          <t>Year 3</t>
+        </is>
+      </c>
+      <c r="B115" s="6" t="inlineStr">
+        <is>
+          <t>B3</t>
+        </is>
+      </c>
+      <c r="C115" s="6" t="inlineStr">
+        <is>
+          <t>physiology</t>
+        </is>
+      </c>
+      <c r="D115" s="6" t="inlineStr">
         <is>
           <t>3</t>
         </is>
       </c>
-      <c r="E83" s="7" t="inlineStr">
+      <c r="E115" s="7" t="inlineStr">
         <is>
           <t>20/11/2025</t>
         </is>
       </c>
-      <c r="F83" s="8" t="inlineStr">
+      <c r="F115" s="8" t="inlineStr">
         <is>
           <t>14:00:00</t>
         </is>
       </c>
-      <c r="G83" s="9" t="n">
+      <c r="G115" s="9" t="n">
         <v>90</v>
       </c>
     </row>

</xml_diff>